<commit_message>
Ini adalah catatan penelitian
</commit_message>
<xml_diff>
--- a/LogBook-NLP-Covid19.xlsx
+++ b/LogBook-NLP-Covid19.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t xml:space="preserve">KK</t>
   </si>
@@ -87,6 +87,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">A. Data
 - Data diambil dari </t>
@@ -97,6 +98,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Twitter
 </t>
@@ -106,6 +108,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Data yang bisa diambil di Twitter hanya pada </t>
     </r>
@@ -115,6 +118,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">satu kali waktu</t>
     </r>
@@ -123,6 +127,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, sebanyak </t>
     </r>
@@ -132,6 +137,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3,200
 </t>
@@ -141,6 +147,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Keywords yang akan diambil: </t>
     </r>
@@ -150,6 +157,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">lockdown
 </t>
@@ -159,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Data diambil berdasarkan bahasa yaitu </t>
     </r>
@@ -168,6 +177,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Melayu</t>
     </r>
@@ -176,6 +186,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">. 
 - Data tidak diambil berdasarkan </t>
@@ -187,6 +198,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Geolocation</t>
     </r>
@@ -195,6 +207,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> yaitu Indonesia karena dikhawatirkan akan banyak tercampur oleh bahasa Inggris</t>
     </r>
@@ -205,6 +218,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1. Apakah data yang diambil </t>
     </r>
@@ -214,6 +228,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dapat mewakili</t>
     </r>
@@ -222,6 +237,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> pendapat orang Indonesia?
 2. </t>
@@ -232,6 +248,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Metode</t>
     </r>
@@ -240,6 +257,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> apa yang digunakan untuk mencari keywords? Agar hal ini ada landasannya ketika menulis di jurnal nanti.
 3. Keywords lockdown bisa ditulis dengan berbagai cara, misalnya: lockdown, lock_down, dll. 
@@ -252,6 +270,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">B. Jurnal
 - Target jurnal adalah </t>
@@ -262,6 +281,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Jurnal Internasional</t>
     </r>
@@ -270,6 +290,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.
 - Perlu dicari Jurnal Internasional yang </t>
@@ -280,6 +301,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">waktu review-nya</t>
     </r>
@@ -288,6 +310,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> cepat, agar sesuai dengan momentum covid19 di Indonesia
 - </t>
@@ -298,6 +321,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Download</t>
     </r>
@@ -306,6 +330,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> template Jurnal
 - Jurnal yang ditarget adalah Jurnal NLP, Sentiment Analysis, Information Science, Text Information</t>
@@ -317,6 +342,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1. Perlu diperhatikan jumlah data yang memadai untuk jurnal Internasional. Karena biasanya Jurnal Internasional meminta dataset dengan satuan </t>
     </r>
@@ -326,6 +352,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ribuan</t>
     </r>
@@ -334,6 +361,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> atau </t>
     </r>
@@ -343,6 +371,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">jutaan</t>
     </r>
@@ -351,6 +380,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">. Apakah dengan data yang kita pakai, bisa mewakili jurnal tersebut?</t>
     </r>
@@ -361,6 +391,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C. Waktu penelitian
 - Direncanakan pada minggu akhir </t>
@@ -371,6 +402,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bulan Maret – April</t>
     </r>
@@ -379,6 +411,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> untuk dapat men</t>
     </r>
@@ -388,6 +421,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">download, cleaning, filtering, dan simulasi dataset
 </t>
@@ -397,6 +431,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Minggu akhir </t>
     </r>
@@ -406,6 +441,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bulan Maret – April</t>
     </r>
@@ -414,6 +450,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> juga direncanakan sudah ada </t>
     </r>
@@ -423,6 +460,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">template Jurnal</t>
     </r>
@@ -431,6 +469,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> yang ditarget
 - Perlu mencari </t>
@@ -441,6 +480,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">research paper</t>
     </r>
@@ -449,6 +489,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> sebagai </t>
     </r>
@@ -458,6 +499,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">landasan</t>
     </r>
@@ -466,6 +508,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> untuk bagian awal di Jurnal yaitu </t>
     </r>
@@ -475,6 +518,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Introduction</t>
     </r>
@@ -483,6 +527,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> dan </t>
     </r>
@@ -492,6 +537,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Related Work
 </t>
@@ -501,6 +547,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">- Setelah simulasi, diharapkan pada </t>
     </r>
@@ -510,6 +557,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bulan Mei</t>
     </r>
@@ -518,6 +566,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> sudah bisa </t>
     </r>
@@ -527,6 +576,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">menyatukan hasil simulasi</t>
     </r>
@@ -535,6 +585,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> dengan </t>
     </r>
@@ -544,6 +595,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">landasan teori</t>
     </r>
@@ -552,6 +604,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, setelah itu melakukan analisis</t>
     </r>
@@ -621,6 +674,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.aclweb.org/anthology/W16-5415.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test jurnal</t>
   </si>
   <si>
     <t xml:space="preserve">Journal Name</t>
@@ -669,11 +725,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -691,64 +748,11 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -756,65 +760,25 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -822,23 +786,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -862,23 +811,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -893,15 +825,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -909,96 +841,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -1013,9 +868,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>283320</xdr:colOff>
+      <xdr:colOff>282960</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1029,7 +884,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7268040" y="3186360"/>
-          <a:ext cx="4297680" cy="2247120"/>
+          <a:ext cx="4298040" cy="2246760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1152,7 +1007,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="66.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="58.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="58.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1205,7 +1060,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1219,10 +1074,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:I8"/>
+  <dimension ref="B4:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1230,11 +1085,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="25.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="20.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="34.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="34.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1315,6 +1170,14 @@
       </c>
       <c r="I8" s="5" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1326,7 +1189,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1359,19 +1222,19 @@
         <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,19 +1242,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1263,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>